<commit_message>
27th April Test Case 10 In progress
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BluestrataTestData.xlsx
+++ b/src/test/resources/testdata/BluestrataTestData.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="172">
   <si>
     <t xml:space="preserve">Test Case </t>
   </si>
@@ -382,13 +382,166 @@
   </si>
   <si>
     <t>PRN Every (x) Hour(s)</t>
+  </si>
+  <si>
+    <t>frequency1</t>
+  </si>
+  <si>
+    <t>Once a Day</t>
+  </si>
+  <si>
+    <t>frequency2</t>
+  </si>
+  <si>
+    <t>frequency3</t>
+  </si>
+  <si>
+    <t>frequency4</t>
+  </si>
+  <si>
+    <t>frequency5</t>
+  </si>
+  <si>
+    <t>frequency6</t>
+  </si>
+  <si>
+    <t>Twice a Day</t>
+  </si>
+  <si>
+    <t>Three Times a Day</t>
+  </si>
+  <si>
+    <t>Four Times a Day</t>
+  </si>
+  <si>
+    <t>Five Times a Day</t>
+  </si>
+  <si>
+    <t>Six Times a Day</t>
+  </si>
+  <si>
+    <t>frequencyTexttype</t>
+  </si>
+  <si>
+    <t>frequencyTexttype1</t>
+  </si>
+  <si>
+    <t>text Box</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>timeInADayTime</t>
+  </si>
+  <si>
+    <t>timeInADayShift</t>
+  </si>
+  <si>
+    <t>Morning</t>
+  </si>
+  <si>
+    <t>08:00 am</t>
+  </si>
+  <si>
+    <t>frequency8</t>
+  </si>
+  <si>
+    <t>Bed Time</t>
+  </si>
+  <si>
+    <t>frequency9</t>
+  </si>
+  <si>
+    <t>frequency10</t>
+  </si>
+  <si>
+    <t>frequency11</t>
+  </si>
+  <si>
+    <t>frequency12</t>
+  </si>
+  <si>
+    <t>frequency13</t>
+  </si>
+  <si>
+    <t>frequency14</t>
+  </si>
+  <si>
+    <t>Every Hour</t>
+  </si>
+  <si>
+    <t>Every Two Hours</t>
+  </si>
+  <si>
+    <t>Every Three Hours</t>
+  </si>
+  <si>
+    <t>Every Four Hours</t>
+  </si>
+  <si>
+    <t>Every Six Hours</t>
+  </si>
+  <si>
+    <t>Every Eight Hours</t>
+  </si>
+  <si>
+    <t>frequency15</t>
+  </si>
+  <si>
+    <t>Every Twelve Hours</t>
+  </si>
+  <si>
+    <t>201332142-1</t>
+  </si>
+  <si>
+    <t>timeInADayShiftBedTime</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>frequency16</t>
+  </si>
+  <si>
+    <t>frequency17</t>
+  </si>
+  <si>
+    <t>frequency18</t>
+  </si>
+  <si>
+    <t>frequency19</t>
+  </si>
+  <si>
+    <t>frequency20</t>
+  </si>
+  <si>
+    <t>frequency21</t>
+  </si>
+  <si>
+    <t>With Meals</t>
+  </si>
+  <si>
+    <t>Before Meals</t>
+  </si>
+  <si>
+    <t>After Meals</t>
+  </si>
+  <si>
+    <t>Before Meals + Bed Time</t>
+  </si>
+  <si>
+    <t>After Meals + Bed Time</t>
+  </si>
+  <si>
+    <t>Only One Time / STAT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,6 +569,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="6">
@@ -463,7 +622,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -502,6 +661,12 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -783,10 +948,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BK29"/>
+  <dimension ref="A1:BU29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC7" sqref="AC7"/>
+    <sheetView tabSelected="1" topLeftCell="AW13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BJ16" sqref="BJ16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -814,12 +979,18 @@
     <col min="27" max="27" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="44" width="9.140625" style="1"/>
+    <col min="30" max="43" width="9.140625" style="1"/>
+    <col min="44" max="44" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="45" max="45" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="9.140625" style="1"/>
+    <col min="46" max="46" width="9.140625" style="1"/>
+    <col min="47" max="48" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="9.140625" style="1"/>
+    <col min="52" max="52" width="11.5703125" style="1" customWidth="1"/>
+    <col min="53" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -829,13 +1000,13 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="6"/>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>118</v>
       </c>
@@ -845,7 +1016,7 @@
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A4" s="13"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
@@ -878,7 +1049,7 @@
       <c r="AD4" s="12"/>
       <c r="AE4" s="11"/>
     </row>
-    <row r="5" spans="1:63" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:73" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -886,7 +1057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
@@ -975,7 +1146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:73" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -1064,7 +1235,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1120,7 +1291,7 @@
       <c r="BA9" s="13"/>
       <c r="BB9" s="13"/>
     </row>
-    <row r="10" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:73" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -1128,7 +1299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:73" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>1</v>
       </c>
@@ -1290,7 +1461,7 @@
       </c>
       <c r="BB11" s="7"/>
     </row>
-    <row r="12" spans="1:63" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:73" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
         <v>118</v>
       </c>
@@ -1451,7 +1622,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A13" s="13"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1507,7 +1678,7 @@
       <c r="BA13" s="13"/>
       <c r="BB13" s="13"/>
     </row>
-    <row r="14" spans="1:63" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:73" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -1515,7 +1686,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:63" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:73" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>1</v>
       </c>
@@ -1646,206 +1817,292 @@
         <v>94</v>
       </c>
       <c r="AR15" s="7" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="AS15" s="7" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="AT15" s="7" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="AU15" s="7" t="s">
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="AV15" s="7" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
       <c r="AW15" s="7" t="s">
-        <v>102</v>
+        <v>127</v>
       </c>
       <c r="AX15" s="7" t="s">
-        <v>104</v>
+        <v>133</v>
       </c>
       <c r="AY15" s="7" t="s">
-        <v>105</v>
+        <v>134</v>
       </c>
       <c r="AZ15" s="7" t="s">
-        <v>111</v>
+        <v>137</v>
       </c>
       <c r="BA15" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="BB15" s="7"/>
-      <c r="BC15" s="7"/>
-      <c r="BD15" s="7"/>
-      <c r="BE15" s="7"/>
-      <c r="BF15" s="7"/>
-      <c r="BG15" s="7"/>
-      <c r="BH15" s="7"/>
-      <c r="BI15" s="7"/>
-      <c r="BJ15" s="7"/>
-      <c r="BK15" s="7"/>
+        <v>138</v>
+      </c>
+      <c r="BB15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="BD15" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="BE15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="BG15" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="BH15" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="BI15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BK15" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="BL15" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="BM15" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="BN15" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="BO15" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="BP15" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="BQ15" s="7"/>
+      <c r="BR15" s="7"/>
+      <c r="BS15" s="7"/>
+      <c r="BT15" s="7"/>
+      <c r="BU15" s="7"/>
     </row>
-    <row r="16" spans="1:63" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="1:73" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="K16" s="1">
+      <c r="K16" s="14">
         <v>5</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="M16" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="N16" s="1" t="s">
+      <c r="N16" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="O16" s="8" t="s">
+      <c r="O16" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="P16" s="1" t="s">
+      <c r="P16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="Q16" s="1" t="s">
+      <c r="Q16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="R16" s="1" t="s">
+      <c r="R16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="S16" s="1" t="s">
+      <c r="S16" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="T16" s="9" t="s">
+      <c r="T16" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="U16" s="8" t="s">
+      <c r="U16" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V16" s="10" t="s">
+      <c r="V16" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="W16" s="1" t="s">
+      <c r="W16" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="X16" s="9" t="s">
+      <c r="X16" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="Y16" s="9" t="s">
+      <c r="Y16" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="Z16" s="8" t="s">
+      <c r="Z16" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="AA16" s="9" t="s">
+      <c r="AA16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AB16" s="8" t="s">
+      <c r="AB16" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="AC16" s="9" t="s">
+      <c r="AC16" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="AD16" s="8" t="s">
+      <c r="AD16" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="AE16" s="9" t="s">
+      <c r="AE16" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="AF16" s="8" t="s">
+      <c r="AF16" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="AG16" s="9" t="s">
+      <c r="AG16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AH16" s="9" t="s">
+      <c r="AH16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AI16" s="9" t="s">
+      <c r="AI16" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="AJ16" s="9" t="s">
+      <c r="AJ16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="AK16" s="9" t="s">
+      <c r="AK16" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="AL16" s="1" t="s">
+      <c r="AL16" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="AM16" s="1" t="s">
+      <c r="AM16" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="AN16" s="9" t="s">
+      <c r="AN16" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="AO16" s="1" t="s">
+      <c r="AO16" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="AP16" s="1" t="s">
+      <c r="AP16" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="AQ16" s="8" t="s">
+      <c r="AQ16" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="AR16" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="AS16" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT16" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="AU16" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="AV16" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW16" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="AX16" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AY16" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="AZ16" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="BA16" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="AR16" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AS16" s="16" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT16" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="AU16" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="AV16" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AW16" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="AX16" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="AY16" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ16" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="BA16" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="BB16" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC16" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="BD16" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="BE16" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="BF16" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="BG16" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="BH16" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="BI16" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="BJ16" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="BK16" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="BL16" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="BM16" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="BN16" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="BO16" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="BP16" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="BQ16" s="14"/>
     </row>
     <row r="18" spans="1:60" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
@@ -1985,16 +2242,36 @@
       <c r="AQ19" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="AR19" s="7"/>
-      <c r="AS19" s="7"/>
-      <c r="AT19" s="7"/>
-      <c r="AU19" s="7"/>
-      <c r="AV19" s="7"/>
-      <c r="AW19" s="7"/>
-      <c r="AX19" s="7"/>
-      <c r="AY19" s="7"/>
-      <c r="AZ19" s="7"/>
-      <c r="BA19" s="7"/>
+      <c r="AR19" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV19" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW19" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX19" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY19" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ19" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA19" s="7" t="s">
+        <v>112</v>
+      </c>
       <c r="BB19" s="7"/>
       <c r="BC19" s="7"/>
       <c r="BD19" s="7"/>
@@ -2133,13 +2410,36 @@
       <c r="AQ20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="AR20" s="8"/>
-      <c r="AS20" s="8"/>
-      <c r="AU20" s="8"/>
-      <c r="AV20" s="8"/>
-      <c r="AW20" s="8"/>
-      <c r="AX20" s="8"/>
-      <c r="AY20" s="8"/>
+      <c r="AR20" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS20" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT20" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AV20" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW20" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX20" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="AY20" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA20" s="1" t="s">
+        <v>113</v>
+      </c>
       <c r="BB20" s="9"/>
       <c r="BC20" s="9"/>
       <c r="BD20" s="9"/>

</xml_diff>

<commit_message>
Test Case Upto 17
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BluestrataTestData.xlsx
+++ b/src/test/resources/testdata/BluestrataTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15825" windowHeight="6510"/>
+    <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="physicianportal" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="188">
   <si>
     <t xml:space="preserve">Test Case </t>
   </si>
@@ -438,9 +438,6 @@
     <t>timeInADayShift</t>
   </si>
   <si>
-    <t>Morning</t>
-  </si>
-  <si>
     <t>08:00 am</t>
   </si>
   <si>
@@ -535,6 +532,57 @@
   </si>
   <si>
     <t>Only One Time / STAT</t>
+  </si>
+  <si>
+    <t>QA14_ResidentOrders_CreateAnOrder</t>
+  </si>
+  <si>
+    <t>medicationType</t>
+  </si>
+  <si>
+    <t>searchMedicationName</t>
+  </si>
+  <si>
+    <t>Search Medications</t>
+  </si>
+  <si>
+    <t>Amox</t>
+  </si>
+  <si>
+    <t>Amoxicillin 875 MG Tablet</t>
+  </si>
+  <si>
+    <t>medicationType1</t>
+  </si>
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>Treatment With Medication</t>
+  </si>
+  <si>
+    <t>Both Ears</t>
+  </si>
+  <si>
+    <t>QA15_ResidentOrders_CreateAnOrderWithFrequencyRoutine</t>
+  </si>
+  <si>
+    <t>Fourth</t>
+  </si>
+  <si>
+    <t>QA17_ResidentOrders_CreateAnOrderWithFrequencyPRN</t>
+  </si>
+  <si>
+    <t>QA16_ResidentOrders_CreateAnOrderWithFrequencyPRNEveryHour</t>
+  </si>
+  <si>
+    <t>201332142</t>
+  </si>
+  <si>
+    <t>EnterValue</t>
+  </si>
+  <si>
+    <t>Evening</t>
   </si>
 </sst>
 </file>
@@ -940,7 +988,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -948,10 +996,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BU29"/>
+  <dimension ref="A1:BU44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BJ16" sqref="BJ16"/>
+    <sheetView tabSelected="1" topLeftCell="AV10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BA16" sqref="BA16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,11 +1052,16 @@
       <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>118</v>
+      <c r="A3" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>185</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
@@ -1462,8 +1515,8 @@
       <c r="BB11" s="7"/>
     </row>
     <row r="12" spans="1:73" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>118</v>
+      <c r="A12" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -1847,49 +1900,49 @@
         <v>138</v>
       </c>
       <c r="BB15" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC15" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="BD15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="BD15" s="7" t="s">
+      <c r="BE15" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="BE15" s="7" t="s">
+      <c r="BF15" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BF15" s="7" t="s">
+      <c r="BG15" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="BG15" s="7" t="s">
+      <c r="BH15" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="BH15" s="7" t="s">
-        <v>148</v>
-      </c>
       <c r="BI15" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BJ15" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BK15" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="BL15" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="BL15" s="7" t="s">
+      <c r="BM15" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="BM15" s="7" t="s">
+      <c r="BN15" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="BN15" s="7" t="s">
+      <c r="BO15" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="BO15" s="7" t="s">
+      <c r="BP15" s="7" t="s">
         <v>164</v>
-      </c>
-      <c r="BP15" s="7" t="s">
-        <v>165</v>
       </c>
       <c r="BQ15" s="7"/>
       <c r="BR15" s="7"/>
@@ -1899,7 +1952,7 @@
     </row>
     <row r="16" spans="1:73" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>23</v>
@@ -2052,55 +2105,55 @@
         <v>136</v>
       </c>
       <c r="AZ16" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BA16" s="16" t="s">
-        <v>139</v>
+        <v>187</v>
       </c>
       <c r="BB16" s="16" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="BC16" s="16" t="s">
+        <v>148</v>
+      </c>
+      <c r="BD16" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="BD16" s="16" t="s">
+      <c r="BE16" s="14" t="s">
         <v>150</v>
       </c>
-      <c r="BE16" s="14" t="s">
+      <c r="BF16" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="BF16" s="16" t="s">
+      <c r="BG16" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="BG16" s="19" t="s">
+      <c r="BH16" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="BH16" s="16" t="s">
-        <v>154</v>
-      </c>
       <c r="BI16" s="16" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BJ16" s="16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="BK16" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="BL16" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="BL16" s="14" t="s">
+      <c r="BM16" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="BM16" s="16" t="s">
+      <c r="BN16" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="BN16" s="16" t="s">
+      <c r="BO16" s="14" t="s">
         <v>169</v>
       </c>
-      <c r="BO16" s="14" t="s">
+      <c r="BP16" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="BP16" s="16" t="s">
-        <v>171</v>
       </c>
       <c r="BQ16" s="14"/>
     </row>
@@ -2281,8 +2334,8 @@
       <c r="BH19" s="7"/>
     </row>
     <row r="20" spans="1:60" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>118</v>
+      <c r="A20" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
@@ -2677,8 +2730,8 @@
       </c>
     </row>
     <row r="24" spans="1:60" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>118</v>
+      <c r="A24" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -3062,8 +3115,8 @@
       </c>
     </row>
     <row r="28" spans="1:60" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>118</v>
+      <c r="A28" s="15" t="s">
+        <v>156</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>23</v>
@@ -3277,6 +3330,1197 @@
       <c r="AZ29" s="13"/>
       <c r="BA29" s="13"/>
     </row>
+    <row r="30" spans="1:60" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="1:60" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I31" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L31" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P31" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q31" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="T31" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="U31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="V31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="W31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="X31" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z31" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA31" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AB31" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC31" s="7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:60" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L32" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="M32" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="N32" s="1">
+        <v>5</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R32" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="S32" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="T32" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="U32" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="V32" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="W32" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="X32" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y32" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Z32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AC32" s="15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="33" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="34" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A34" s="5"/>
+      <c r="B34" s="5"/>
+    </row>
+    <row r="35" spans="1:54" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P35" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q35" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S35" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T35" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y35" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB35" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC35" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH35" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK35" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL35" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM35" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN35" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO35" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP35" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR35" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS35" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT35" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU35" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV35" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW35" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX35" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY35" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ35" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA35" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB35" s="7"/>
+    </row>
+    <row r="36" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A36" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K36" s="1">
+        <v>5</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O36" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P36" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T36" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="U36" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="V36" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="W36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X36" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y36" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z36" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB36" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC36" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD36" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE36" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF36" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI36" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ36" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK36" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL36" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN36" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ36" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR36" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS36" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT36" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU36" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AV36" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW36" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX36" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY36" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA36" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="38" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+    </row>
+    <row r="39" spans="1:54" ht="75" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K39" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L39" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N39" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O39" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P39" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R39" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T39" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA39" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC39" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD39" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE39" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF39" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG39" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH39" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI39" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ39" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK39" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL39" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM39" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN39" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO39" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP39" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ39" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR39" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS39" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT39" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU39" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV39" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW39" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX39" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY39" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ39" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA39" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB39" s="7"/>
+    </row>
+    <row r="40" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J40" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K40" s="1">
+        <v>5</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P40" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T40" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="U40" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="V40" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="W40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X40" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y40" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA40" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB40" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC40" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD40" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE40" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF40" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG40" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH40" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI40" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ40" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK40" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM40" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN40" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP40" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR40" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS40" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT40" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AV40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW40" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX40" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY40" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA40" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="41" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+    </row>
+    <row r="43" spans="1:54" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O43" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="P43" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q43" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R43" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S43" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T43" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA43" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB43" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AD43" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE43" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF43" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG43" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AH43" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI43" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="AK43" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="AL43" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AM43" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AN43" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AO43" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AP43" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AQ43" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="AR43" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="AS43" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="AT43" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="AU43" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="AV43" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="AW43" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="AX43" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="AY43" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="AZ43" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA43" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB43" s="7"/>
+    </row>
+    <row r="44" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" s="15" t="s">
+        <v>156</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="J44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="K44" s="1">
+        <v>5</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M44" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="O44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="P44" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="S44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="T44" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="U44" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="V44" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="W44" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X44" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y44" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="Z44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AA44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB44" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC44" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD44" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE44" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="AF44" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="AG44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI44" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ44" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK44" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL44" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM44" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN44" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AO44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP44" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ44" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AR44" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="AS44" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="AT44" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="AU44" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="AV44" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="AW44" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="AX44" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="AY44" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ44" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA44" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Upto Test Case 23
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BluestrataTestData.xlsx
+++ b/src/test/resources/testdata/BluestrataTestData.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2505" windowWidth="15825" windowHeight="6450"/>
+    <workbookView xWindow="0" yWindow="2565" windowWidth="15825" windowHeight="6390"/>
   </bookViews>
   <sheets>
     <sheet name="physicianportal" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1010" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1390" uniqueCount="217">
   <si>
     <t xml:space="preserve">Test Case </t>
   </si>
@@ -375,9 +375,6 @@
     <t>PRN</t>
   </si>
   <si>
-    <t>201332147-1</t>
-  </si>
-  <si>
     <t>QA13_ResidentOrders_CreateAnOrderWithFrequencyPRNEveryHour</t>
   </si>
   <si>
@@ -583,6 +580,96 @@
   </si>
   <si>
     <t>Evening</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>type8</t>
+  </si>
+  <si>
+    <t>type9</t>
+  </si>
+  <si>
+    <t>frequencyType1</t>
+  </si>
+  <si>
+    <t>frequencyType2</t>
+  </si>
+  <si>
+    <t>frequencyType3</t>
+  </si>
+  <si>
+    <t>QA18_ResidentOrders_CreateAnOrderWithFrequencyPRN</t>
+  </si>
+  <si>
+    <t>ResidentNo</t>
+  </si>
+  <si>
+    <t>WithoutMed</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>QA19_ViewAndModifyAnOrder_ViaOrderSets</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>physicianType1</t>
+  </si>
+  <si>
+    <t>ReceivedByType1</t>
+  </si>
+  <si>
+    <t>REYHANI, SEAN</t>
+  </si>
+  <si>
+    <t>word, Bobby</t>
+  </si>
+  <si>
+    <t>discontinueForCorrection</t>
+  </si>
+  <si>
+    <t>copyOrder</t>
+  </si>
+  <si>
+    <t>dcMessage</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>2010064-1</t>
+  </si>
+  <si>
+    <t>administeredBy1</t>
+  </si>
+  <si>
+    <t>RN</t>
+  </si>
+  <si>
+    <t>discontinueForCorrection1</t>
+  </si>
+  <si>
+    <t>copyOrder1</t>
+  </si>
+  <si>
+    <t>dcMessage1</t>
+  </si>
+  <si>
+    <t>Amoxicillin 400 MG/5ML Suspension Reconstituted</t>
+  </si>
+  <si>
+    <t>QA20_VerifyAnOrder_ViaOrderSetsOrCreateAnOrder</t>
+  </si>
+  <si>
+    <t>QA21_VerifyAndModifyAnOrder_ViaOrderSetsOrCreateAnOrder</t>
+  </si>
+  <si>
+    <t>description1</t>
   </si>
 </sst>
 </file>
@@ -988,7 +1075,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -996,10 +1083,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BU44"/>
+  <dimension ref="A1:BU60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AV10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BA16" sqref="BA16"/>
+    <sheetView tabSelected="1" topLeftCell="AP54" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BB59" sqref="BB59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,9 +1114,12 @@
     <col min="27" max="27" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="11.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="43" width="9.140625" style="1"/>
+    <col min="30" max="30" width="9.140625" style="1"/>
+    <col min="31" max="31" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="42" width="9.140625" style="1"/>
+    <col min="43" max="43" width="14.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="20.85546875" style="1" customWidth="1"/>
     <col min="46" max="46" width="9.140625" style="1"/>
     <col min="47" max="48" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="16.140625" style="1" bestFit="1" customWidth="1"/>
@@ -1053,15 +1143,15 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:73" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2"/>
@@ -1284,8 +1374,8 @@
       <c r="AB7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AC7" s="9" t="s">
-        <v>118</v>
+      <c r="AC7" s="15" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:73" x14ac:dyDescent="0.25">
@@ -1516,7 +1606,7 @@
     </row>
     <row r="12" spans="1:73" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>23</v>
@@ -1870,79 +1960,79 @@
         <v>94</v>
       </c>
       <c r="AR15" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="AS15" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="AT15" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="AT15" s="7" t="s">
+      <c r="AU15" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="AU15" s="7" t="s">
+      <c r="AV15" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="AV15" s="7" t="s">
+      <c r="AW15" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="AW15" s="7" t="s">
-        <v>127</v>
-      </c>
       <c r="AX15" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="AY15" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="AY15" s="7" t="s">
-        <v>134</v>
-      </c>
       <c r="AZ15" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="BA15" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="BA15" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="BB15" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BC15" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD15" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="BD15" s="7" t="s">
+      <c r="BE15" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="BE15" s="7" t="s">
+      <c r="BF15" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="BF15" s="7" t="s">
+      <c r="BG15" s="7" t="s">
         <v>145</v>
       </c>
-      <c r="BG15" s="7" t="s">
+      <c r="BH15" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="BH15" s="7" t="s">
-        <v>147</v>
-      </c>
       <c r="BI15" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="BJ15" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="BK15" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="BL15" s="7" t="s">
         <v>159</v>
       </c>
-      <c r="BL15" s="7" t="s">
+      <c r="BM15" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="BM15" s="7" t="s">
+      <c r="BN15" s="7" t="s">
         <v>161</v>
       </c>
-      <c r="BN15" s="7" t="s">
+      <c r="BO15" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="BO15" s="7" t="s">
+      <c r="BP15" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="BP15" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="BQ15" s="7"/>
       <c r="BR15" s="7"/>
@@ -1952,7 +2042,7 @@
     </row>
     <row r="16" spans="1:73" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>23</v>
@@ -2081,79 +2171,79 @@
         <v>85</v>
       </c>
       <c r="AR16" s="16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AS16" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AT16" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="AT16" s="14" t="s">
+      <c r="AU16" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="AU16" s="16" t="s">
+      <c r="AV16" s="16" t="s">
         <v>130</v>
       </c>
-      <c r="AV16" s="16" t="s">
+      <c r="AW16" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="AW16" s="16" t="s">
-        <v>132</v>
-      </c>
       <c r="AX16" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="AY16" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="AY16" s="16" t="s">
-        <v>136</v>
-      </c>
       <c r="AZ16" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="BA16" s="16" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BB16" s="16" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BC16" s="16" t="s">
+        <v>147</v>
+      </c>
+      <c r="BD16" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="BD16" s="16" t="s">
+      <c r="BE16" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="BE16" s="14" t="s">
+      <c r="BF16" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="BF16" s="16" t="s">
+      <c r="BG16" s="19" t="s">
         <v>151</v>
       </c>
-      <c r="BG16" s="19" t="s">
+      <c r="BH16" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="BH16" s="16" t="s">
-        <v>153</v>
-      </c>
       <c r="BI16" s="16" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="BJ16" s="16" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="BK16" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="BL16" s="14" t="s">
         <v>165</v>
       </c>
-      <c r="BL16" s="14" t="s">
+      <c r="BM16" s="16" t="s">
         <v>166</v>
       </c>
-      <c r="BM16" s="16" t="s">
+      <c r="BN16" s="16" t="s">
         <v>167</v>
       </c>
-      <c r="BN16" s="16" t="s">
+      <c r="BO16" s="14" t="s">
         <v>168</v>
       </c>
-      <c r="BO16" s="14" t="s">
+      <c r="BP16" s="16" t="s">
         <v>169</v>
-      </c>
-      <c r="BP16" s="16" t="s">
-        <v>170</v>
       </c>
       <c r="BQ16" s="14"/>
     </row>
@@ -2335,7 +2425,7 @@
     </row>
     <row r="20" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>23</v>
@@ -2731,7 +2821,7 @@
     </row>
     <row r="24" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -2950,7 +3040,7 @@
         <v>0</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:60" ht="75" x14ac:dyDescent="0.25">
@@ -3116,7 +3206,7 @@
     </row>
     <row r="28" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>23</v>
@@ -3176,7 +3266,7 @@
         <v>88</v>
       </c>
       <c r="U28" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V28" s="10" t="s">
         <v>89</v>
@@ -3335,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:60" ht="45" x14ac:dyDescent="0.25">
@@ -3346,13 +3436,13 @@
         <v>5</v>
       </c>
       <c r="C31" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>9</v>
@@ -3429,19 +3519,19 @@
     </row>
     <row r="32" spans="1:60" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="C32" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>28</v>
@@ -3456,7 +3546,7 @@
         <v>30</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>34</v>
@@ -3501,7 +3591,7 @@
         <v>53</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Z32" s="1" t="s">
         <v>34</v>
@@ -3513,7 +3603,7 @@
         <v>34</v>
       </c>
       <c r="AC32" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:54" ht="30" x14ac:dyDescent="0.25">
@@ -3521,7 +3611,7 @@
         <v>0</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:54" x14ac:dyDescent="0.25">
@@ -3692,13 +3782,13 @@
     </row>
     <row r="36" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B36" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C36" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>25</v>
@@ -3716,7 +3806,7 @@
         <v>29</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J36" s="9" t="s">
         <v>54</v>
@@ -3737,7 +3827,7 @@
         <v>40</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q36" s="1" t="s">
         <v>34</v>
@@ -3839,7 +3929,7 @@
         <v>110</v>
       </c>
       <c r="AX36" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AY36" s="8" t="s">
         <v>107</v>
@@ -3856,7 +3946,7 @@
         <v>0</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:54" x14ac:dyDescent="0.25">
@@ -4027,13 +4117,13 @@
     </row>
     <row r="40" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B40" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>25</v>
@@ -4051,7 +4141,7 @@
         <v>29</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J40" s="9" t="s">
         <v>54</v>
@@ -4072,7 +4162,7 @@
         <v>40</v>
       </c>
       <c r="P40" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q40" s="1" t="s">
         <v>34</v>
@@ -4087,7 +4177,7 @@
         <v>88</v>
       </c>
       <c r="U40" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="V40" s="10" t="s">
         <v>89</v>
@@ -4174,7 +4264,7 @@
         <v>110</v>
       </c>
       <c r="AX40" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AY40" s="8" t="s">
         <v>107</v>
@@ -4191,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="42" spans="1:54" x14ac:dyDescent="0.25">
@@ -4362,13 +4452,13 @@
     </row>
     <row r="44" spans="1:54" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>179</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>25</v>
@@ -4386,7 +4476,7 @@
         <v>29</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="J44" s="9" t="s">
         <v>54</v>
@@ -4407,7 +4497,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="Q44" s="1" t="s">
         <v>34</v>
@@ -4509,7 +4599,7 @@
         <v>110</v>
       </c>
       <c r="AX44" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AY44" s="8" t="s">
         <v>107</v>
@@ -4519,6 +4609,1204 @@
       </c>
       <c r="BA44" s="1" t="s">
         <v>113</v>
+      </c>
+    </row>
+    <row r="45" spans="1:54" ht="30" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:54" x14ac:dyDescent="0.25">
+      <c r="A46" s="5"/>
+      <c r="B46" s="5"/>
+    </row>
+    <row r="47" spans="1:54" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="P47" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q47" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T47" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y47" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z47" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA47" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB47" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC47" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD47" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE47" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF47" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG47" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI47" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK47" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL47" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM47" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN47" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:54" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="L48" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M48" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O48" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q48" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="R48" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S48" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="T48" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="U48" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V48" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W48" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="X48" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y48" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z48" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA48" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB48" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD48" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE48" s="15" t="s">
+        <v>155</v>
+      </c>
+      <c r="AF48" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG48" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH48" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI48" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ48" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK48" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM48" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN48" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:59" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A50" s="5"/>
+      <c r="B50" s="5"/>
+    </row>
+    <row r="51" spans="1:59" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K51" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N51" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="O51" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="P51" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q51" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T51" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y51" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z51" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA51" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB51" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC51" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD51" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE51" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF51" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG51" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH51" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ51" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK51" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL51" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN51" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO51" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP51" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ51" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR51" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS51" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT51" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU51" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV51" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW51" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX51" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY51" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AZ51" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="BA51" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB51" s="6"/>
+      <c r="BC51" s="6"/>
+      <c r="BD51" s="6"/>
+      <c r="BE51" s="6"/>
+      <c r="BF51" s="6"/>
+      <c r="BG51" s="6"/>
+    </row>
+    <row r="52" spans="1:59" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K52" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O52" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P52" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q52" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="R52" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S52" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="T52" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="U52" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V52" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W52" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="X52" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y52" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z52" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA52" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB52" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD52" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE52" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF52" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG52" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH52" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI52" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ52" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK52" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO52" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP52" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ52" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="AR52" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS52" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW52" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY52" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AZ52" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA52" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:59" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="54" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A54" s="5"/>
+      <c r="B54" s="5"/>
+    </row>
+    <row r="55" spans="1:59" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B55" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L55" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M55" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="O55" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T55" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y55" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z55" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA55" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB55" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC55" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD55" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE55" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF55" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG55" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI55" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ55" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK55" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL55" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM55" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN55" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO55" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56" spans="1:59" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M56" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N56" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O56" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P56" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q56" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="R56" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S56" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="T56" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="U56" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V56" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W56" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="X56" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y56" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z56" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA56" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB56" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD56" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE56" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF56" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG56" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH56" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI56" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ56" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK56" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN56" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO56" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:59" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:59" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="5"/>
+    </row>
+    <row r="59" spans="1:59" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B59" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I59" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="L59" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M59" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="P59" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q59" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="T59" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="V59" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="W59" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="X59" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y59" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z59" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="AA59" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB59" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC59" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="AD59" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="AE59" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="AF59" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG59" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH59" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="AI59" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="AJ59" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="AK59" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL59" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="AM59" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="AN59" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO59" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="AP59" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AQ59" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR59" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="AS59" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AT59" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="AU59" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="AV59" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW59" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX59" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="AY59" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="AZ59" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="BA59" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="BB59" s="7" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:59" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="J60" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K60" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="L60" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="M60" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="N60" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="O60" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="P60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q60" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="R60" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="S60" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="T60" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="U60" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="V60" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="W60" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="X60" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y60" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="Z60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA60" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB60" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="AC60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AE60" s="15" t="s">
+        <v>207</v>
+      </c>
+      <c r="AF60" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AG60" s="1">
+        <v>5</v>
+      </c>
+      <c r="AH60" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI60" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AJ60" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AK60" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AM60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AN60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AO60" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP60" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ60" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="AR60" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS60" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="AT60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AV60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AW60" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AY60" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="AZ60" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="BA60" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="BB60" s="15" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All Updates Test Case
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/BluestrataTestData.xlsx
+++ b/src/test/resources/testdata/BluestrataTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="660" windowWidth="13395" windowHeight="3120" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="660" windowWidth="13395" windowHeight="3120" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="physicianportal" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8755" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8757" uniqueCount="364">
   <si>
     <t xml:space="preserve">Test Case </t>
   </si>
@@ -1106,13 +1106,16 @@
   </si>
   <si>
     <t>Gen_QA213_HelpMenuWith_HelpSiteAbout</t>
+  </si>
+  <si>
+    <t>Amoxicill-Clarithro-Lansopraz Miscellaneous</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1131,6 +1134,12 @@
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1165,7 +1174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1210,6 +1219,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1513,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR42"/>
   <sheetViews>
-    <sheetView topLeftCell="AZ38" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:BR42"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6827,7 +6837,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:70" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>230</v>
       </c>
@@ -6861,8 +6871,8 @@
       <c r="K26" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="L26" s="8" t="s">
-        <v>200</v>
+      <c r="L26" s="26" t="s">
+        <v>363</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>183</v>
@@ -6922,7 +6932,7 @@
         <v>107</v>
       </c>
       <c r="AF26" s="6" t="s">
-        <v>329</v>
+        <v>9</v>
       </c>
       <c r="AG26" s="9" t="s">
         <v>48</v>
@@ -10441,8 +10451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR42"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:BR42"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15750,7 +15760,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:70" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:70" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>260</v>
       </c>
@@ -15784,8 +15794,8 @@
       <c r="K26" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="L26" s="8" t="s">
-        <v>200</v>
+      <c r="L26" s="26" t="s">
+        <v>363</v>
       </c>
       <c r="M26" s="7" t="s">
         <v>183</v>
@@ -18391,8 +18401,8 @@
       <c r="AF38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AG38" s="6">
-        <v>20120951</v>
+      <c r="AG38" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="AH38" s="9" t="s">
         <v>48</v>
@@ -18815,8 +18825,8 @@
       <c r="AF40" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="AG40" s="6">
-        <v>20120951</v>
+      <c r="AG40" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="AH40" s="9" t="s">
         <v>48</v>
@@ -19363,7 +19373,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BR26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A25" sqref="A25:BR26"/>
     </sheetView>
   </sheetViews>

</xml_diff>